<commit_message>
Se agregan resultados de pruebas manuales - Testing
</commit_message>
<xml_diff>
--- a/docs/Testing-web (2).xlsx
+++ b/docs/Testing-web (2).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4981FF4F-1B46-4381-9250-C95B2415EFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0DD09CB-A21E-438D-8EB5-29078AD90C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -232,9 +232,6 @@
     <t xml:space="preserve">Cada botón debe dirigir al usuario a la página correspondiente </t>
   </si>
   <si>
-    <t xml:space="preserve">La navegabilidad se observa fluida e intuitiva. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Al accionar en el boton registrarme se deja constancia en la base de datos de MySQL el usuario correctamente creado. </t>
   </si>
   <si>
@@ -244,12 +241,6 @@
     <t xml:space="preserve">Al no completar alguno de los datos no se habilita el boton registrarme, por lo tanto el usuario no puede ser creado. </t>
   </si>
   <si>
-    <t>Al colocar un usuario incorrecto y contraseña correcta, no se observan mensajes validadores de error, pero el estado de la solicitud arroja un mensaje 400.</t>
-  </si>
-  <si>
-    <t>Al colocar un usuario correcto y contraseña erronea, no se observan mensajes validadores de error, pero el estado de la solicitud arroja un mensaje 400.</t>
-  </si>
-  <si>
     <t>Al cerrar la sesion el usuario es redirigido a la pagina de login.</t>
   </si>
   <si>
@@ -266,6 +257,27 @@
   </si>
   <si>
     <t xml:space="preserve">Se realiza la pruba de los botones en el menu y todos redireccionan a sus páginas correspondientes </t>
+  </si>
+  <si>
+    <t>Ingresar el usuario con formato incorrecto de email</t>
+  </si>
+  <si>
+    <t>El usuario debe haber cargado su usuario con el formato incorrecto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema alertar que el formato es incorrecto o no corresponde. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El ingresar un usuario (es un email), sin @ o sin su parte final ".com" el frontend dice que el formato no es válido. Lo cual es lo esperado. </t>
+  </si>
+  <si>
+    <t>Al colocar un usuario incorrecto y contraseña correcta,  se observan mensajes validadores de error, el sistema dice arroja un mensaje "Credenciales inválidas"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al colocar un usuario incorrecto y contraseña correcta,  se observan mensajes validadores de error, el sistema dice arroja un mensaje "Credenciales inválidas" Además el log de python muestra un estado 400. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La navegabilidad se observa fluida e intuitiva. No se muestran lentitudes o cargas de elementos inesperados. </t>
   </si>
 </sst>
 </file>
@@ -295,7 +307,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +330,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -374,31 +392,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -426,6 +429,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,19 +666,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H997"/>
+  <dimension ref="A1:H998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="17" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="12" customWidth="1"/>
     <col min="5" max="5" width="34.85546875" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" customWidth="1"/>
     <col min="7" max="7" width="36.42578125" customWidth="1"/>
@@ -671,10 +692,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -691,324 +712,347 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="10">
         <v>3</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>68</v>
+      <c r="H2" s="18" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="15">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>70</v>
+      <c r="H3" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="9" t="s">
-        <v>69</v>
+      <c r="A4" s="14"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="10">
         <v>2</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="10">
+        <v>2</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="10">
+        <v>2</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="15">
-        <v>1</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="15">
-        <v>2</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="15">
-        <v>1</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="15">
-        <v>1</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C11" s="10">
         <v>2</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="10">
+        <v>3</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="11">
+        <v>2</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="15">
-        <v>2</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="15">
-        <v>2</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="15">
-        <v>3</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="16">
-        <v>2</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1991,15 +2035,16 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>